<commit_message>
fixed file data read.
</commit_message>
<xml_diff>
--- a/exceldoc/ApiDoc01.xlsx
+++ b/exceldoc/ApiDoc01.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="120">
   <si>
     <t>リクエスト種別</t>
     <rPh sb="5" eb="7">
@@ -799,6 +799,215 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>呼出パラメータ名2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出パラメータ名3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出パラメータ名4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出パラメータ名5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出パラメータ名1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値パラメータ名1</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値パラメータ名2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値パラメータ名3</t>
+    <rPh sb="1" eb="2">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値パラメータ名4</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値パラメータ名5</t>
+  </si>
+  <si>
+    <t>呼出物理名1</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出物理名2</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出物理名3</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出物理名4</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出物理名5</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出型1</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出型2</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出型3</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出型4</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>呼出型5</t>
+    <rPh sb="0" eb="2">
+      <t>ヨビダ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値物理名1</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>○</t>
+  </si>
+  <si>
+    <t>戻値物理名2</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値物理名3</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値物理名4</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値物理名5</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>チ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://localhost:8080/test</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻値型1</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1186,14 +1395,14 @@
   <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.125" customWidth="1"/>
     <col min="2" max="3" width="21.125" customWidth="1"/>
-    <col min="4" max="4" width="21.75" customWidth="1"/>
+    <col min="4" max="4" width="42.875" customWidth="1"/>
     <col min="5" max="5" width="22.375" customWidth="1"/>
     <col min="6" max="6" width="26.625" customWidth="1"/>
   </cols>
@@ -1243,7 +1452,9 @@
       <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -1268,48 +1479,88 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -1335,48 +1586,88 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
       <c r="E22" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
       <c r="E24" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="1">
+        <v>4</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5</v>
+      </c>
       <c r="E26" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.15"/>

</xml_diff>